<commit_message>
Add chi-sq GOF test to sample table
</commit_message>
<xml_diff>
--- a/Model building/Sample.xlsx
+++ b/Model building/Sample.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\pc\Dokumenter\MSc\Thesis\Model building\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{66A009D3-562C-4303-BFE4-260175D9BD23}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5C7440B-4497-40BE-A67F-73FFB932FA7B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E6D6AC90-8912-4EE9-AF92-D9A0275D085E}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="56">
   <si>
     <t>Country</t>
   </si>
@@ -181,6 +181,18 @@
   </si>
   <si>
     <t>students each school sent</t>
+  </si>
+  <si>
+    <t>chi-sq test of goodness of fit</t>
+  </si>
+  <si>
+    <t>chisq</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>&lt;.001</t>
   </si>
 </sst>
 </file>
@@ -245,7 +257,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -274,12 +286,6 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -291,6 +297,15 @@
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -606,10 +621,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED437C5F-40C3-44A8-80D3-2B4C225B7A23}">
-  <dimension ref="A1:N23"/>
+  <dimension ref="A1:N26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O11" sqref="O11"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -639,20 +654,20 @@
         <v>0</v>
       </c>
       <c r="D1" s="7"/>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="F1" s="11"/>
+      <c r="F1" s="14"/>
       <c r="G1" s="7"/>
-      <c r="H1" s="11" t="s">
+      <c r="H1" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="I1" s="11"/>
+      <c r="I1" s="14"/>
       <c r="J1" s="7"/>
-      <c r="K1" s="10" t="s">
+      <c r="K1" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="L1" s="10"/>
+      <c r="L1" s="15"/>
       <c r="N1" s="1" t="s">
         <v>50</v>
       </c>
@@ -706,7 +721,7 @@
         <v>595</v>
       </c>
       <c r="F3" s="3">
-        <f>E3/E$23</f>
+        <f t="shared" ref="F3:F22" si="0">E3/E$23</f>
         <v>8.9730055798522099E-2</v>
       </c>
       <c r="G3" s="3"/>
@@ -714,7 +729,7 @@
         <v>8310</v>
       </c>
       <c r="I3" s="3">
-        <f>H3/H$23</f>
+        <f t="shared" ref="I3:I22" si="1">H3/H$23</f>
         <v>7.7546145088744148E-2</v>
       </c>
       <c r="J3" s="3"/>
@@ -722,10 +737,10 @@
         <v>4045</v>
       </c>
       <c r="L3" s="3">
-        <f>K3/H3</f>
+        <f t="shared" ref="L3:L22" si="2">K3/H3</f>
         <v>0.48676293622141997</v>
       </c>
-      <c r="N3" s="15">
+      <c r="N3" s="13">
         <f>H3/E3</f>
         <v>13.966386554621849</v>
       </c>
@@ -744,7 +759,7 @@
         <v>558</v>
       </c>
       <c r="F4" s="3">
-        <f>E4/E$23</f>
+        <f t="shared" si="0"/>
         <v>8.4150203589202235E-2</v>
       </c>
       <c r="G4" s="3"/>
@@ -752,7 +767,7 @@
         <v>9124</v>
       </c>
       <c r="I4" s="3">
-        <f>H4/H$23</f>
+        <f t="shared" si="1"/>
         <v>8.5142121274332322E-2</v>
       </c>
       <c r="J4" s="3"/>
@@ -760,11 +775,11 @@
         <v>4601</v>
       </c>
       <c r="L4" s="3">
-        <f>K4/H4</f>
+        <f t="shared" si="2"/>
         <v>0.50427444103463392</v>
       </c>
-      <c r="N4" s="15">
-        <f t="shared" ref="N4:N22" si="0">H4/E4</f>
+      <c r="N4" s="13">
+        <f t="shared" ref="N4:N22" si="3">H4/E4</f>
         <v>16.351254480286737</v>
       </c>
     </row>
@@ -782,7 +797,7 @@
         <v>539</v>
       </c>
       <c r="F5" s="3">
-        <f>E5/E$23</f>
+        <f t="shared" si="0"/>
         <v>8.1284874076308244E-2</v>
       </c>
       <c r="G5" s="3"/>
@@ -790,7 +805,7 @@
         <v>9182</v>
       </c>
       <c r="I5" s="3">
-        <f>H5/H$23</f>
+        <f t="shared" si="1"/>
         <v>8.5683357906720672E-2</v>
       </c>
       <c r="J5" s="3"/>
@@ -798,11 +813,11 @@
         <v>4706</v>
       </c>
       <c r="L5" s="3">
-        <f>K5/H5</f>
+        <f t="shared" si="2"/>
         <v>0.5125245044652581</v>
       </c>
-      <c r="N5" s="15">
-        <f t="shared" si="0"/>
+      <c r="N5" s="13">
+        <f t="shared" si="3"/>
         <v>17.035250463821892</v>
       </c>
     </row>
@@ -820,7 +835,7 @@
         <v>492</v>
       </c>
       <c r="F6" s="3">
-        <f>E6/E$23</f>
+        <f t="shared" si="0"/>
         <v>7.4196953702307347E-2</v>
       </c>
       <c r="G6" s="3"/>
@@ -828,7 +843,7 @@
         <v>7762</v>
       </c>
       <c r="I6" s="3">
-        <f>H6/H$23</f>
+        <f t="shared" si="1"/>
         <v>7.2432392079281829E-2</v>
       </c>
       <c r="J6" s="3"/>
@@ -836,11 +851,11 @@
         <v>3858</v>
       </c>
       <c r="L6" s="3">
-        <f>K6/H6</f>
+        <f t="shared" si="2"/>
         <v>0.49703684617366656</v>
       </c>
-      <c r="N6" s="15">
-        <f t="shared" si="0"/>
+      <c r="N6" s="13">
+        <f t="shared" si="3"/>
         <v>15.776422764227643</v>
       </c>
     </row>
@@ -858,7 +873,7 @@
         <v>491</v>
       </c>
       <c r="F7" s="3">
-        <f>E7/E$23</f>
+        <f t="shared" si="0"/>
         <v>7.4046146885839242E-2</v>
       </c>
       <c r="G7" s="3"/>
@@ -866,7 +881,7 @@
         <v>9361</v>
       </c>
       <c r="I7" s="3">
-        <f>H7/H$23</f>
+        <f t="shared" si="1"/>
         <v>8.7353726134264009E-2</v>
       </c>
       <c r="J7" s="3"/>
@@ -874,11 +889,11 @@
         <v>4695</v>
       </c>
       <c r="L7" s="3">
-        <f>K7/H7</f>
+        <f t="shared" si="2"/>
         <v>0.50154897980984936</v>
       </c>
-      <c r="N7" s="15">
-        <f t="shared" si="0"/>
+      <c r="N7" s="13">
+        <f t="shared" si="3"/>
         <v>19.065173116089614</v>
       </c>
     </row>
@@ -896,7 +911,7 @@
         <v>395</v>
       </c>
       <c r="F8" s="3">
-        <f>E8/E$23</f>
+        <f t="shared" si="0"/>
         <v>5.9568692504901224E-2</v>
       </c>
       <c r="G8" s="3"/>
@@ -904,7 +919,7 @@
         <v>7132</v>
       </c>
       <c r="I8" s="3">
-        <f>H8/H$23</f>
+        <f t="shared" si="1"/>
         <v>6.6553442451615305E-2</v>
       </c>
       <c r="J8" s="3"/>
@@ -912,11 +927,11 @@
         <v>3454</v>
       </c>
       <c r="L8" s="3">
-        <f>K8/H8</f>
+        <f t="shared" si="2"/>
         <v>0.484296130117779</v>
       </c>
-      <c r="N8" s="15">
-        <f t="shared" si="0"/>
+      <c r="N8" s="13">
+        <f t="shared" si="3"/>
         <v>18.055696202531646</v>
       </c>
     </row>
@@ -934,7 +949,7 @@
         <v>357</v>
       </c>
       <c r="F9" s="3">
-        <f>E9/E$23</f>
+        <f t="shared" si="0"/>
         <v>5.3838033479113256E-2</v>
       </c>
       <c r="G9" s="3"/>
@@ -942,7 +957,7 @@
         <v>3411</v>
       </c>
       <c r="I9" s="3">
-        <f>H9/H$23</f>
+        <f t="shared" si="1"/>
         <v>3.1830312984080178E-2</v>
       </c>
       <c r="J9" s="3"/>
@@ -950,11 +965,11 @@
         <v>1683</v>
       </c>
       <c r="L9" s="3">
-        <f>K9/H9</f>
+        <f t="shared" si="2"/>
         <v>0.49340369393139843</v>
       </c>
-      <c r="N9" s="15">
-        <f t="shared" si="0"/>
+      <c r="N9" s="13">
+        <f t="shared" si="3"/>
         <v>9.5546218487394956</v>
       </c>
     </row>
@@ -972,7 +987,7 @@
         <v>349</v>
       </c>
       <c r="F10" s="3">
-        <f>E10/E$23</f>
+        <f t="shared" si="0"/>
         <v>5.2631578947368418E-2</v>
       </c>
       <c r="G10" s="3"/>
@@ -980,7 +995,7 @@
         <v>4075</v>
       </c>
       <c r="I10" s="3">
-        <f>H10/H$23</f>
+        <f t="shared" si="1"/>
         <v>3.8026539258319184E-2</v>
       </c>
       <c r="J10" s="3"/>
@@ -988,11 +1003,11 @@
         <v>2060</v>
       </c>
       <c r="L10" s="3">
-        <f>K10/H10</f>
+        <f t="shared" si="2"/>
         <v>0.505521472392638</v>
       </c>
-      <c r="N10" s="15">
-        <f t="shared" si="0"/>
+      <c r="N10" s="13">
+        <f t="shared" si="3"/>
         <v>11.676217765042979</v>
       </c>
     </row>
@@ -1010,7 +1025,7 @@
         <v>337</v>
       </c>
       <c r="F11" s="3">
-        <f>E11/E$23</f>
+        <f t="shared" si="0"/>
         <v>5.0821897149751168E-2</v>
       </c>
       <c r="G11" s="3"/>
@@ -1018,7 +1033,7 @@
         <v>4732</v>
       </c>
       <c r="I11" s="3">
-        <f>H11/H$23</f>
+        <f t="shared" si="1"/>
         <v>4.4157443870028554E-2</v>
       </c>
       <c r="J11" s="3"/>
@@ -1026,11 +1041,11 @@
         <v>2390</v>
       </c>
       <c r="L11" s="3">
-        <f>K11/H11</f>
+        <f t="shared" si="2"/>
         <v>0.50507185122569742</v>
       </c>
-      <c r="N11" s="15">
-        <f t="shared" si="0"/>
+      <c r="N11" s="13">
+        <f t="shared" si="3"/>
         <v>14.041543026706231</v>
       </c>
     </row>
@@ -1048,7 +1063,7 @@
         <v>319</v>
       </c>
       <c r="F12" s="3">
-        <f>E12/E$23</f>
+        <f t="shared" si="0"/>
         <v>4.8107374453325288E-2</v>
       </c>
       <c r="G12" s="3"/>
@@ -1056,7 +1071,7 @@
         <v>4320</v>
       </c>
       <c r="I12" s="3">
-        <f>H12/H$23</f>
+        <f t="shared" si="1"/>
         <v>4.0312797446856161E-2</v>
       </c>
       <c r="J12" s="3"/>
@@ -1064,11 +1079,11 @@
         <v>2239</v>
       </c>
       <c r="L12" s="3">
-        <f>K12/H12</f>
+        <f t="shared" si="2"/>
         <v>0.51828703703703705</v>
       </c>
-      <c r="N12" s="15">
-        <f t="shared" si="0"/>
+      <c r="N12" s="13">
+        <f t="shared" si="3"/>
         <v>13.542319749216301</v>
       </c>
     </row>
@@ -1086,7 +1101,7 @@
         <v>307</v>
       </c>
       <c r="F13" s="3">
-        <f>E13/E$23</f>
+        <f t="shared" si="0"/>
         <v>4.6297692655708038E-2</v>
       </c>
       <c r="G13" s="3"/>
@@ -1094,7 +1109,7 @@
         <v>3151</v>
       </c>
       <c r="I13" s="3">
-        <f>H13/H$23</f>
+        <f t="shared" si="1"/>
         <v>2.9404079804408279E-2</v>
       </c>
       <c r="J13" s="3"/>
@@ -1102,11 +1117,11 @@
         <v>1587</v>
       </c>
       <c r="L13" s="3">
-        <f>K13/H13</f>
+        <f t="shared" si="2"/>
         <v>0.5036496350364964</v>
       </c>
-      <c r="N13" s="15">
-        <f t="shared" si="0"/>
+      <c r="N13" s="13">
+        <f t="shared" si="3"/>
         <v>10.26384364820847</v>
       </c>
     </row>
@@ -1124,7 +1139,7 @@
         <v>276</v>
       </c>
       <c r="F14" s="3">
-        <f>E14/E$23</f>
+        <f t="shared" si="0"/>
         <v>4.1622681345196803E-2</v>
       </c>
       <c r="G14" s="3"/>
@@ -1132,7 +1147,7 @@
         <v>4568</v>
       </c>
       <c r="I14" s="3">
-        <f>H14/H$23</f>
+        <f t="shared" si="1"/>
         <v>4.2627050633620128E-2</v>
       </c>
       <c r="J14" s="3"/>
@@ -1140,11 +1155,11 @@
         <v>2320</v>
       </c>
       <c r="L14" s="3">
-        <f>K14/H14</f>
+        <f t="shared" si="2"/>
         <v>0.50788091068301222</v>
       </c>
-      <c r="N14" s="15">
-        <f t="shared" si="0"/>
+      <c r="N14" s="13">
+        <f t="shared" si="3"/>
         <v>16.55072463768116</v>
       </c>
     </row>
@@ -1162,7 +1177,7 @@
         <v>251</v>
       </c>
       <c r="F15" s="3">
-        <f>E15/E$23</f>
+        <f t="shared" si="0"/>
         <v>3.7852510933494191E-2</v>
       </c>
       <c r="G15" s="3"/>
@@ -1170,7 +1185,7 @@
         <v>4482</v>
       </c>
       <c r="I15" s="3">
-        <f>H15/H$23</f>
+        <f t="shared" si="1"/>
         <v>4.1824527351113271E-2</v>
       </c>
       <c r="J15" s="3"/>
@@ -1178,11 +1193,11 @@
         <v>2254</v>
       </c>
       <c r="L15" s="3">
-        <f>K15/H15</f>
+        <f t="shared" si="2"/>
         <v>0.50290049085229804</v>
       </c>
-      <c r="N15" s="15">
-        <f t="shared" si="0"/>
+      <c r="N15" s="13">
+        <f t="shared" si="3"/>
         <v>17.856573705179283</v>
       </c>
     </row>
@@ -1200,7 +1215,7 @@
         <v>235</v>
       </c>
       <c r="F16" s="3">
-        <f>E16/E$23</f>
+        <f t="shared" si="0"/>
         <v>3.5439601870004521E-2</v>
       </c>
       <c r="G16" s="3"/>
@@ -1208,7 +1223,7 @@
         <v>4294</v>
       </c>
       <c r="I16" s="3">
-        <f>H16/H$23</f>
+        <f t="shared" si="1"/>
         <v>4.0070174128888969E-2</v>
       </c>
       <c r="J16" s="3"/>
@@ -1216,11 +1231,11 @@
         <v>2080</v>
       </c>
       <c r="L16" s="3">
-        <f>K16/H16</f>
+        <f t="shared" si="2"/>
         <v>0.48439683278993945</v>
       </c>
-      <c r="N16" s="15">
-        <f t="shared" si="0"/>
+      <c r="N16" s="13">
+        <f t="shared" si="3"/>
         <v>18.272340425531915</v>
       </c>
     </row>
@@ -1238,7 +1253,7 @@
         <v>229</v>
       </c>
       <c r="F17" s="3">
-        <f>E17/E$23</f>
+        <f t="shared" si="0"/>
         <v>3.4534760971195899E-2</v>
       </c>
       <c r="G17" s="3"/>
@@ -1246,7 +1261,7 @@
         <v>4166</v>
       </c>
       <c r="I17" s="3">
-        <f>H17/H$23</f>
+        <f t="shared" si="1"/>
         <v>3.8875720871204347E-2</v>
       </c>
       <c r="J17" s="3"/>
@@ -1254,11 +1269,11 @@
         <v>2080</v>
       </c>
       <c r="L17" s="3">
-        <f>K17/H17</f>
+        <f t="shared" si="2"/>
         <v>0.49927988478156504</v>
       </c>
-      <c r="N17" s="15">
-        <f t="shared" si="0"/>
+      <c r="N17" s="13">
+        <f t="shared" si="3"/>
         <v>18.192139737991265</v>
       </c>
     </row>
@@ -1276,7 +1291,7 @@
         <v>204</v>
       </c>
       <c r="F18" s="3">
-        <f>E18/E$23</f>
+        <f t="shared" si="0"/>
         <v>3.076459055949329E-2</v>
       </c>
       <c r="G18" s="3"/>
@@ -1284,7 +1299,7 @@
         <v>4328</v>
       </c>
       <c r="I18" s="3">
-        <f>H18/H$23</f>
+        <f t="shared" si="1"/>
         <v>4.038745077546145E-2</v>
       </c>
       <c r="J18" s="3"/>
@@ -1292,11 +1307,11 @@
         <v>2199</v>
       </c>
       <c r="L18" s="3">
-        <f>K18/H18</f>
+        <f t="shared" si="2"/>
         <v>0.50808687615526804</v>
       </c>
-      <c r="N18" s="15">
-        <f t="shared" si="0"/>
+      <c r="N18" s="13">
+        <f t="shared" si="3"/>
         <v>21.215686274509803</v>
       </c>
     </row>
@@ -1314,7 +1329,7 @@
         <v>197</v>
       </c>
       <c r="F19" s="3">
-        <f>E19/E$23</f>
+        <f t="shared" si="0"/>
         <v>2.970894284421656E-2</v>
       </c>
       <c r="G19" s="3"/>
@@ -1322,7 +1337,7 @@
         <v>4110</v>
       </c>
       <c r="I19" s="3">
-        <f>H19/H$23</f>
+        <f t="shared" si="1"/>
         <v>3.8353147570967319E-2</v>
       </c>
       <c r="J19" s="3"/>
@@ -1330,11 +1345,11 @@
         <v>2147</v>
       </c>
       <c r="L19" s="3">
-        <f>K19/H19</f>
+        <f t="shared" si="2"/>
         <v>0.52238442822384423</v>
       </c>
-      <c r="N19" s="15">
-        <f t="shared" si="0"/>
+      <c r="N19" s="13">
+        <f t="shared" si="3"/>
         <v>20.862944162436548</v>
       </c>
     </row>
@@ -1352,7 +1367,7 @@
         <v>186</v>
       </c>
       <c r="F20" s="3">
-        <f>E20/E$23</f>
+        <f t="shared" si="0"/>
         <v>2.8050067863067411E-2</v>
       </c>
       <c r="G20" s="3"/>
@@ -1360,7 +1375,7 @@
         <v>3874</v>
       </c>
       <c r="I20" s="3">
-        <f>H20/H$23</f>
+        <f t="shared" si="1"/>
         <v>3.6150874377111286E-2</v>
       </c>
       <c r="J20" s="3"/>
@@ -1368,11 +1383,11 @@
         <v>1951</v>
       </c>
       <c r="L20" s="3">
-        <f>K20/H20</f>
+        <f t="shared" si="2"/>
         <v>0.50361383582860098</v>
       </c>
-      <c r="N20" s="15">
-        <f t="shared" si="0"/>
+      <c r="N20" s="13">
+        <f t="shared" si="3"/>
         <v>20.827956989247312</v>
       </c>
     </row>
@@ -1383,35 +1398,35 @@
       <c r="B21" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="C21" s="13" t="s">
+      <c r="C21" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13">
+      <c r="D21" s="11"/>
+      <c r="E21" s="11">
         <v>163</v>
       </c>
-      <c r="F21" s="14">
-        <f>E21/E$23</f>
+      <c r="F21" s="12">
+        <f t="shared" si="0"/>
         <v>2.4581511084301011E-2</v>
       </c>
-      <c r="G21" s="14"/>
-      <c r="H21" s="13">
+      <c r="G21" s="12"/>
+      <c r="H21" s="11">
         <v>3738</v>
       </c>
-      <c r="I21" s="14">
-        <f>H21/H$23</f>
+      <c r="I21" s="12">
+        <f t="shared" si="1"/>
         <v>3.4881767790821375E-2</v>
       </c>
-      <c r="J21" s="14"/>
-      <c r="K21" s="13">
+      <c r="J21" s="12"/>
+      <c r="K21" s="11">
         <v>1871</v>
       </c>
-      <c r="L21" s="14">
-        <f>K21/H21</f>
+      <c r="L21" s="12">
+        <f t="shared" si="2"/>
         <v>0.50053504547886574</v>
       </c>
-      <c r="N21" s="15">
-        <f t="shared" si="0"/>
+      <c r="N21" s="13">
+        <f t="shared" si="3"/>
         <v>22.932515337423315</v>
       </c>
     </row>
@@ -1430,7 +1445,7 @@
         <v>151</v>
       </c>
       <c r="F22" s="9">
-        <f>E22/E$23</f>
+        <f t="shared" si="0"/>
         <v>2.2771829286683757E-2</v>
       </c>
       <c r="G22" s="9"/>
@@ -1438,7 +1453,7 @@
         <v>3042</v>
       </c>
       <c r="I22" s="9">
-        <f>H22/H$23</f>
+        <f t="shared" si="1"/>
         <v>2.8386928202161214E-2</v>
       </c>
       <c r="J22" s="9"/>
@@ -1446,11 +1461,11 @@
         <v>1549</v>
       </c>
       <c r="L22" s="9">
-        <f>K22/H22</f>
+        <f t="shared" si="2"/>
         <v>0.50920447074293229</v>
       </c>
-      <c r="N22" s="15">
-        <f t="shared" si="0"/>
+      <c r="N22" s="13">
+        <f t="shared" si="3"/>
         <v>20.14569536423841</v>
       </c>
     </row>
@@ -1463,7 +1478,7 @@
         <f>SUM(E3:E22)</f>
         <v>6631</v>
       </c>
-      <c r="F23" s="12">
+      <c r="F23" s="10">
         <f>SUM(F3:F22)</f>
         <v>0.99999999999999989</v>
       </c>
@@ -1472,7 +1487,7 @@
         <f>SUM(H3:H22)</f>
         <v>107162</v>
       </c>
-      <c r="I23" s="12">
+      <c r="I23" s="10">
         <f>SUM(I3:I22)</f>
         <v>1.0000000000000002</v>
       </c>
@@ -1482,22 +1497,78 @@
         <v>53769</v>
       </c>
       <c r="L23" s="3">
-        <f t="shared" ref="L4:L23" si="1">K23/H23</f>
+        <f t="shared" ref="L23" si="4">K23/H23</f>
         <v>0.50175435322222428</v>
       </c>
-      <c r="N23" s="15">
+      <c r="N23" s="13">
         <f>H23/E23</f>
         <v>16.160760066355</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+      <c r="F24" s="10"/>
+      <c r="G24" s="3"/>
+      <c r="I24" s="10"/>
+      <c r="J24" s="3"/>
+      <c r="L24" s="3"/>
+      <c r="N24" s="13"/>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="E25" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="I25" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="K25" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="L25" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A26" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="B26" s="16"/>
+      <c r="C26" s="16"/>
+      <c r="E26" s="2">
+        <v>1105.8</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="H26" s="2">
+        <v>16984</v>
+      </c>
+      <c r="I26" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="K26" s="2">
+        <v>20.9</v>
+      </c>
+      <c r="L26" s="2">
+        <v>0.34</v>
       </c>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:L22">
     <sortCondition descending="1" ref="F3:F22"/>
   </sortState>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="H1:I1"/>
     <mergeCell ref="K1:L1"/>
+    <mergeCell ref="A26:C26"/>
   </mergeCells>
   <conditionalFormatting sqref="F3:F22">
     <cfRule type="dataBar" priority="5">
@@ -1541,7 +1612,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N3:N23">
+  <conditionalFormatting sqref="N3:N24">
     <cfRule type="dataBar" priority="1">
       <dataBar>
         <cfvo type="min"/>
@@ -1601,7 +1672,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>N3:N23</xm:sqref>
+          <xm:sqref>N3:N24</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>